<commit_message>
script stub with Workbook Template
</commit_message>
<xml_diff>
--- a/bt_expense/Expenses.xlsx
+++ b/bt_expense/Expenses.xlsx
@@ -9,14 +9,24 @@
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
     <sheet name="Setup" sheetId="2" r:id="rId2"/>
-    <sheet name="Lookups" sheetId="3" r:id="rId3"/>
+    <sheet name="Projects" sheetId="3" r:id="rId3"/>
+    <sheet name="Categories" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="category">ExpenseEntries[Expense Category]</definedName>
+    <definedName name="cost">ExpenseEntries[Cost]</definedName>
+    <definedName name="date">ExpenseEntries[Date]</definedName>
+    <definedName name="note">ExpenseEntries[Notes]</definedName>
+    <definedName name="project">ExpenseEntries[Project]</definedName>
+    <definedName name="project_name_lk">Project_lookup[Project Name]</definedName>
+    <definedName name="projectsid_lk">Project_lookup[projectsid]</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>User Id</t>
   </si>
@@ -39,9 +49,6 @@
     <t>firm_name_here</t>
   </si>
   <si>
-    <t>user_name/id_here</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -61,6 +68,42 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Project A</t>
+  </si>
+  <si>
+    <t>Project B</t>
+  </si>
+  <si>
+    <t>Project C</t>
+  </si>
+  <si>
+    <t>Project D</t>
+  </si>
+  <si>
+    <t>Meals</t>
+  </si>
+  <si>
+    <t>Airfare</t>
+  </si>
+  <si>
+    <t>Lodging</t>
+  </si>
+  <si>
+    <t>Ground Transportation</t>
+  </si>
+  <si>
+    <t>user_id_here</t>
+  </si>
+  <si>
+    <t>Project E</t>
   </si>
 </sst>
 </file>
@@ -70,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,16 +140,37 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -114,12 +178,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -141,12 +251,87 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -154,6 +339,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ExpenseEntries" displayName="ExpenseEntries" ref="A1:G31" totalsRowShown="0">
+  <autoFilter ref="A1:G31"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Project" dataDxfId="7"/>
+    <tableColumn id="2" name="Expense Category" dataDxfId="6"/>
+    <tableColumn id="3" name="Date" dataDxfId="5">
+      <calculatedColumnFormula>NOW()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Cost" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Notes"/>
+    <tableColumn id="6" name="projectsid" dataDxfId="3">
+      <calculatedColumnFormula>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="catsid" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Project_lookup" displayName="Project_lookup" ref="A1:B51" totalsRowShown="0">
+  <autoFilter ref="A1:B51"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Project Name"/>
+    <tableColumn id="2" name="projectsid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Cat_lookup" displayName="Cat_lookup" ref="A1:B11" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:B11"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Category Name"/>
+    <tableColumn id="2" name="catsid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,50 +672,556 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6"/>
+    <col min="1" max="1" width="28.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="4"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="10"/>
+    <col min="6" max="6" width="14.42578125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43115</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6">
+        <v>43116</v>
+      </c>
+      <c r="F3" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6">
+        <v>43117</v>
+      </c>
+      <c r="F4" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6">
+        <v>43118</v>
+      </c>
+      <c r="F5" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="9" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43119</v>
+      </c>
+      <c r="F6" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="G6" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6">
+        <v>43120</v>
+      </c>
+      <c r="F7" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G7" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="8"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43121</v>
+      </c>
+      <c r="F8" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G8" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6">
+        <v>43122</v>
+      </c>
+      <c r="F9" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6">
+        <v>43123</v>
+      </c>
+      <c r="F10" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="15">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="C11" s="6">
+        <f t="shared" ref="C2:C31" ca="1" si="0">NOW()</f>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F11" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G11" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="C12" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F12" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G12" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="C13" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F13" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G13" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="C14" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F14" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G14" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="C15" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F15" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G15" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="C16" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F16" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G16" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="C17" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F17" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G17" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="C18" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F18" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G18" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="C19" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F19" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G19" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="C20" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F20" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G20" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="C21" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F21" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G21" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="C22" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F22" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G22" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="C23" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F23" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G23" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="C24" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F24" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G24" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="C25" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F25" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G25" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="C26" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F26" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G26" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="C27" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F27" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G27" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="C28" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F28" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G28" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="C29" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F29" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G29" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="C30" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F30" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G30" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="C31" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43121.800431018521</v>
+      </c>
+      <c r="F31" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Project]], Project_lookup[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G31" s="15" t="e">
+        <f>VLOOKUP(ExpenseEntries[[#This Row],[Expense Category]], Cat_lookup[],2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Projects!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Projects!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B31</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -495,7 +1230,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -543,12 +1278,133 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>